<commit_message>
added files for updated srs ctrl version.
</commit_message>
<xml_diff>
--- a/board/capMeasBOM.xlsx
+++ b/board/capMeasBOM.xlsx
@@ -7,24 +7,147 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Depreciated" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>q`</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Ref Des</t>
+  </si>
+  <si>
+    <t>Cost/Unit</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10K0</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=112&amp;FV=fff40001%2Cfff800e9%2Cfffc02e2%2C80002%2Cc0001%2C1c0002%2C1c0003%2C1c00c5%2C1c0124%2C400005%2C440067&amp;k=RESISTORS&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>AD5640BRJZ-1500RL7</t>
+  </si>
+  <si>
+    <t>Mfg</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/AD5640BRJZ-1500RL7/AD5640BRJZ-1500RL7CT-ND/3471192</t>
+  </si>
+  <si>
+    <t>IC DAC 14BIT SPI/SRL SOT23-8</t>
+  </si>
+  <si>
+    <t>SOT23-8</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>GRM32ER71H106KA12L</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 50V 10% X7R 1210</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?v=490&amp;FV=fff40002%2Cfff8000b%2Cc0001%2Cc0002%2Cc0003%2Cc0004%2C1c0002%2C340045%2C380020%2C400005%2C400006%2C400008%2C440005%2C440012%2C11401c5&amp;k=CERAMIC+CAPACITOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>GRM188R71H104KA93D</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM188R71H104KA93D/490-1519-1-ND/587854</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=73131-5013</t>
+  </si>
+  <si>
+    <t>CONN BNC JACK STR 50 OHM PCB</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>C1, C3</t>
+  </si>
+  <si>
+    <t>C2, C4</t>
+  </si>
+  <si>
+    <t>TLV341AIDBVR</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 2.3MHZ RRO SOT23-6</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/TLV341AIDBVR/296-17680-1-ND/716532</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -52,8 +175,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,17 +490,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E24"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2">
+        <v>7.13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1210</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f>A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>731315013</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.56</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>603</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new file for bom and added mcu to mcuio page.
</commit_message>
<xml_diff>
--- a/board/capMeasBOM.xlsx
+++ b/board/capMeasBOM.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="23520" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
-    <sheet name="Depreciated" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>Item #</t>
   </si>
@@ -50,9 +49,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv1=112&amp;FV=fff40001%2Cfff800e9%2Cfffc02e2%2C80002%2Cc0001%2C1c0002%2C1c0003%2C1c00c5%2C1c0124%2C400005%2C440067&amp;k=RESISTORS&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>AD5640BRJZ-1500RL7</t>
   </si>
   <si>
@@ -107,15 +103,6 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>C1, C3</t>
-  </si>
-  <si>
-    <t>C2, C4</t>
-  </si>
-  <si>
     <t>TLV341AIDBVR</t>
   </si>
   <si>
@@ -132,6 +119,102 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/TLV341AIDBVR/296-17680-1-ND/716532</t>
+  </si>
+  <si>
+    <t>Qnt</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>C1, C3, C5</t>
+  </si>
+  <si>
+    <t>C2, C4, C6</t>
+  </si>
+  <si>
+    <t>LED SUPER RED CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>LTST-C170KRKT</t>
+  </si>
+  <si>
+    <t>Lite-On</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=LTST-C170KRKT&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RMCF0603FT100R/RMCF0603FT100RCT-ND/1942965</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100R</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>SIL05-1A85-76D4K</t>
+  </si>
+  <si>
+    <t>RELAY REED SPST 1A 5V</t>
+  </si>
+  <si>
+    <t>Merder</t>
+  </si>
+  <si>
+    <t>LS1</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=sil05-1a85-76d4k</t>
+  </si>
+  <si>
+    <t>AD817ARZ-REEL7</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 50MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/AD817ARZ-REEL7/AD817ARZ-REEL7CT-ND/4162142</t>
+  </si>
+  <si>
+    <t>U3, U4</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=112&amp;FV=fff40001%2Cfff800e9%2Cfffc02e2%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=RESISTOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>RMCF0603FT22K0</t>
+  </si>
+  <si>
+    <t>RES SMD 22K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=320&amp;FV=fff40001%2Cfff800e9%2Cfffc02e2%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=RESISTOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>ADC for transimp circuit</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100K</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RMCF0603FT100K/RMCF0603FT100KCT-ND/1943118</t>
   </si>
 </sst>
 </file>
@@ -490,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,14 +585,15 @@
     <col min="2" max="2" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,232 +604,388 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
         <v>7.13</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A8" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1210</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1210</v>
-      </c>
-      <c r="H3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>731315013</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.56</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2">
-        <v>2.56</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <f>A5+1</f>
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" ref="A9:A12" si="1">A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>9.09</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f>A12+1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4.92</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f>A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>603</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>